<commit_message>
Excel y txt con los valores de la tercera medicion (30-5)
</commit_message>
<xml_diff>
--- a/TP2B/GraficoDeMediciones - Desordenados.xlsx
+++ b/TP2B/GraficoDeMediciones - Desordenados.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enzo.almiron\Desktop\TP2B\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="8055" windowHeight="7230"/>
   </bookViews>
@@ -49,8 +44,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,25 +172,13 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="es-AR"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -212,102 +195,77 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Elementales!$A$3:$A$15</c:f>
+              <c:f>Elementales!$A$3:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>20000</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>30000</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>40000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>50000</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>60000</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>70000</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>80000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>90000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>120000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>140000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>160000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>180000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>200000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Elementales!$B$3:$B$15</c:f>
+              <c:f>Elementales!$B$3:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>263</c:v>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>680</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>593</c:v>
+                  <c:v>1460</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1050</c:v>
+                  <c:v>2140</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1647</c:v>
+                  <c:v>4830</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2366</c:v>
+                  <c:v>8530</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3214</c:v>
+                  <c:v>13340</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4208</c:v>
+                  <c:v>19300</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5328</c:v>
+                  <c:v>26420</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9469</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>12899</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>16850</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>21318</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>26318</c:v>
+                  <c:v>34260</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-1EFB-4C9D-A06B-6208419670D8}"/>
             </c:ext>
@@ -329,102 +287,77 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Elementales!$A$3:$A$15</c:f>
+              <c:f>Elementales!$A$3:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>20000</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>30000</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>40000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>50000</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>60000</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>70000</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>80000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>90000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>120000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>140000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>160000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>180000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>200000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Elementales!$C$3:$C$15</c:f>
+              <c:f>Elementales!$C$3:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>129</c:v>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>492</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>287</c:v>
+                  <c:v>1372</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>511</c:v>
+                  <c:v>2094</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>799</c:v>
+                  <c:v>4763</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1147</c:v>
+                  <c:v>8308</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1550</c:v>
+                  <c:v>13234</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2035</c:v>
+                  <c:v>18858</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2568</c:v>
+                  <c:v>25660</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4588</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6233</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>8124</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>10294</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12732</c:v>
+                  <c:v>33470</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-1EFB-4C9D-A06B-6208419670D8}"/>
             </c:ext>
@@ -446,146 +379,128 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Elementales!$A$3:$A$15</c:f>
+              <c:f>Elementales!$A$3:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>20000</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>30000</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>40000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>50000</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>60000</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>70000</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>80000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>90000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>120000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>140000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>160000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>180000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>200000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Elementales!$D$3:$D$15</c:f>
+              <c:f>Elementales!$D$3:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>196</c:v>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>530</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>438</c:v>
+                  <c:v>880</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>779</c:v>
+                  <c:v>1310</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1215</c:v>
+                  <c:v>2940</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1749</c:v>
+                  <c:v>5230</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2386</c:v>
+                  <c:v>8120</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3119</c:v>
+                  <c:v>11720</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3955</c:v>
+                  <c:v>16030</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7043</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9599</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>12527</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>15856</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>19553</c:v>
+                  <c:v>20920</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-1EFB-4C9D-A06B-6208419670D8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="101506432"/>
-        <c:axId val="101504896"/>
+        <c:dLbls/>
+        <c:axId val="60484608"/>
+        <c:axId val="60568320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101506432"/>
+        <c:axId val="60484608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101504896"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="es-ES"/>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="60568320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101504896"/>
+        <c:axId val="60568320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101506432"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="es-ES"/>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="60484608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -593,40 +508,36 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="es-ES"/>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="es-AR"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -643,102 +554,83 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'No Elementales'!$A$3:$A$15</c:f>
+              <c:f>'No Elementales'!$A$3:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>20000</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30000</c:v>
+                  <c:v>2000000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40000</c:v>
+                  <c:v>3000000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50000</c:v>
+                  <c:v>4000000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>60000</c:v>
+                  <c:v>5000000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>70000</c:v>
+                  <c:v>6000000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>80000</c:v>
+                  <c:v>7000000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>90000</c:v>
+                  <c:v>8000000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>120000</c:v>
+                  <c:v>9000000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>140000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>160000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>180000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>200000</c:v>
+                  <c:v>10000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'No Elementales'!$B$3:$B$15</c:f>
+              <c:f>'No Elementales'!$B$3:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>901</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2111</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>3641</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>4981</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>6441</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>8091</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>9831</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>11381</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>13561</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>14</c:v>
+                  <c:v>17031</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-CC4B-46DD-B12E-B7D7B6C8BDBB}"/>
             </c:ext>
@@ -760,102 +652,83 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'No Elementales'!$A$3:$A$15</c:f>
+              <c:f>'No Elementales'!$A$3:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>20000</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30000</c:v>
+                  <c:v>2000000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40000</c:v>
+                  <c:v>3000000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50000</c:v>
+                  <c:v>4000000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>60000</c:v>
+                  <c:v>5000000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>70000</c:v>
+                  <c:v>6000000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>80000</c:v>
+                  <c:v>7000000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>90000</c:v>
+                  <c:v>8000000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>120000</c:v>
+                  <c:v>9000000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>140000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>160000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>180000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>200000</c:v>
+                  <c:v>10000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'No Elementales'!$C$3:$C$15</c:f>
+              <c:f>'No Elementales'!$C$3:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>221</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>451</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>701</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>941</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1172</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1431</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1671</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1901</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>2141</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>2421</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-CC4B-46DD-B12E-B7D7B6C8BDBB}"/>
             </c:ext>
@@ -877,146 +750,134 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'No Elementales'!$A$3:$A$15</c:f>
+              <c:f>'No Elementales'!$A$3:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>20000</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30000</c:v>
+                  <c:v>2000000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40000</c:v>
+                  <c:v>3000000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50000</c:v>
+                  <c:v>4000000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>60000</c:v>
+                  <c:v>5000000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>70000</c:v>
+                  <c:v>6000000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>80000</c:v>
+                  <c:v>7000000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>90000</c:v>
+                  <c:v>8000000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>120000</c:v>
+                  <c:v>9000000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>140000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>160000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>180000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>200000</c:v>
+                  <c:v>10000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'No Elementales'!$D$3:$D$15</c:f>
+              <c:f>'No Elementales'!$D$3:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>791</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>1611</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2521</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>3431</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>4341</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>5509</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>6383</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>7181</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>7921</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>14</c:v>
+                  <c:v>9133</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-CC4B-46DD-B12E-B7D7B6C8BDBB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="49071616"/>
-        <c:axId val="49070080"/>
+        <c:dLbls/>
+        <c:axId val="60640256"/>
+        <c:axId val="60650240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="49071616"/>
+        <c:axId val="60640256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49070080"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="es-ES"/>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="60650240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="49070080"/>
+        <c:axId val="60650240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49071616"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="es-ES"/>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="60640256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1024,15 +885,23 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="es-ES"/>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1043,15 +912,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>76197</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:colOff>57147</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>133349</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1080,13 +949,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>133349</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1109,7 +978,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1151,7 +1020,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1183,10 +1052,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1218,7 +1086,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1394,14 +1261,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J18" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.28515625" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
@@ -1409,7 +1276,7 @@
     <col min="4" max="4" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -1419,7 +1286,7 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="5"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -1431,186 +1298,144 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
+        <v>10000</v>
+      </c>
+      <c r="B3" s="1">
+        <v>680</v>
+      </c>
+      <c r="C3" s="1">
+        <v>492</v>
+      </c>
+      <c r="D3" s="1">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>16384</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1460</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1372</v>
+      </c>
+      <c r="D4" s="1">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
         <v>20000</v>
       </c>
-      <c r="B3" s="1">
-        <v>263</v>
-      </c>
-      <c r="C3" s="1">
-        <v>129</v>
-      </c>
-      <c r="D3" s="1">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="B5" s="1">
+        <v>2140</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2094</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
         <v>30000</v>
       </c>
-      <c r="B4" s="1">
-        <v>593</v>
-      </c>
-      <c r="C4" s="1">
-        <v>287</v>
-      </c>
-      <c r="D4" s="1">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="B6" s="1">
+        <v>4830</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4763</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2940</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
         <v>40000</v>
       </c>
-      <c r="B5" s="1">
-        <v>1050</v>
-      </c>
-      <c r="C5" s="1">
-        <v>511</v>
-      </c>
-      <c r="D5" s="1">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="B7" s="1">
+        <v>8530</v>
+      </c>
+      <c r="C7" s="1">
+        <v>8308</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
         <v>50000</v>
       </c>
-      <c r="B6" s="1">
-        <v>1647</v>
-      </c>
-      <c r="C6" s="1">
-        <v>799</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1215</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="B8" s="1">
+        <v>13340</v>
+      </c>
+      <c r="C8" s="1">
+        <v>13234</v>
+      </c>
+      <c r="D8" s="1">
+        <v>8120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
         <v>60000</v>
       </c>
-      <c r="B7" s="1">
-        <v>2366</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1147</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1749</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="B9" s="1">
+        <v>19300</v>
+      </c>
+      <c r="C9" s="1">
+        <v>18858</v>
+      </c>
+      <c r="D9" s="1">
+        <v>11720</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
         <v>70000</v>
       </c>
-      <c r="B8" s="1">
-        <v>3214</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1550</v>
-      </c>
-      <c r="D8" s="1">
-        <v>2386</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="B10" s="1">
+        <v>26420</v>
+      </c>
+      <c r="C10" s="1">
+        <v>25660</v>
+      </c>
+      <c r="D10" s="1">
+        <v>16030</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
         <v>80000</v>
       </c>
-      <c r="B9" s="1">
-        <v>4208</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2035</v>
-      </c>
-      <c r="D9" s="1">
-        <v>3119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="B11" s="1">
+        <v>34260</v>
+      </c>
+      <c r="C11" s="1">
+        <v>33470</v>
+      </c>
+      <c r="D11" s="1">
+        <v>20920</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1">
         <v>90000</v>
       </c>
-      <c r="B10" s="1">
-        <v>5328</v>
-      </c>
-      <c r="C10" s="1">
-        <v>2568</v>
-      </c>
-      <c r="D10" s="1">
-        <v>3955</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>120000</v>
-      </c>
-      <c r="B11" s="1">
-        <v>9469</v>
-      </c>
-      <c r="C11" s="1">
-        <v>4588</v>
-      </c>
-      <c r="D11" s="1">
-        <v>7043</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>140000</v>
-      </c>
       <c r="B12" s="1">
-        <v>12899</v>
+        <v>43340</v>
       </c>
       <c r="C12" s="1">
-        <v>6233</v>
+        <v>42603</v>
       </c>
       <c r="D12" s="1">
-        <v>9599</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>160000</v>
-      </c>
-      <c r="B13" s="1">
-        <v>16850</v>
-      </c>
-      <c r="C13" s="1">
-        <v>8124</v>
-      </c>
-      <c r="D13" s="1">
-        <v>12527</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>180000</v>
-      </c>
-      <c r="B14" s="1">
-        <v>21318</v>
-      </c>
-      <c r="C14" s="1">
-        <v>10294</v>
-      </c>
-      <c r="D14" s="1">
-        <v>15856</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>200000</v>
-      </c>
-      <c r="B15" s="1">
-        <v>26318</v>
-      </c>
-      <c r="C15" s="1">
-        <v>12732</v>
-      </c>
-      <c r="D15" s="1">
-        <v>19553</v>
+        <v>26600</v>
       </c>
     </row>
   </sheetData>
@@ -1628,20 +1453,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -1651,7 +1476,7 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="5"/>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -1663,186 +1488,144 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
-        <v>20000</v>
+        <v>1000000</v>
       </c>
       <c r="B3" s="1">
-        <v>2</v>
+        <v>901</v>
       </c>
       <c r="C3" s="1">
-        <v>0</v>
+        <v>221</v>
       </c>
       <c r="D3" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
-        <v>30000</v>
+        <v>2000000</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>2111</v>
       </c>
       <c r="C4" s="1">
-        <v>0</v>
+        <v>451</v>
       </c>
       <c r="D4" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1611</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
-        <v>40000</v>
+        <v>3000000</v>
       </c>
       <c r="B5" s="1">
-        <v>2</v>
+        <v>3641</v>
       </c>
       <c r="C5" s="1">
-        <v>0</v>
+        <v>701</v>
       </c>
       <c r="D5" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2521</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
-        <v>50000</v>
+        <v>4000000</v>
       </c>
       <c r="B6" s="1">
-        <v>3</v>
+        <v>4981</v>
       </c>
       <c r="C6" s="1">
-        <v>0</v>
+        <v>941</v>
       </c>
       <c r="D6" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3431</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
-        <v>60000</v>
+        <v>5000000</v>
       </c>
       <c r="B7" s="1">
-        <v>3</v>
+        <v>6441</v>
       </c>
       <c r="C7" s="1">
-        <v>0</v>
+        <v>1172</v>
       </c>
       <c r="D7" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4341</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
-        <v>70000</v>
+        <v>6000000</v>
       </c>
       <c r="B8" s="1">
-        <v>5</v>
+        <v>8091</v>
       </c>
       <c r="C8" s="1">
-        <v>0</v>
+        <v>1431</v>
       </c>
       <c r="D8" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5509</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
-        <v>80000</v>
+        <v>7000000</v>
       </c>
       <c r="B9" s="1">
-        <v>6</v>
+        <v>9831</v>
       </c>
       <c r="C9" s="1">
-        <v>0</v>
+        <v>1671</v>
       </c>
       <c r="D9" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6383</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
-        <v>90000</v>
+        <v>8000000</v>
       </c>
       <c r="B10" s="1">
-        <v>6</v>
+        <v>11381</v>
       </c>
       <c r="C10" s="1">
-        <v>0</v>
+        <v>1901</v>
       </c>
       <c r="D10" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
-        <v>120000</v>
+        <v>9000000</v>
       </c>
       <c r="B11" s="1">
-        <v>8</v>
+        <v>13561</v>
       </c>
       <c r="C11" s="1">
-        <v>0</v>
+        <v>2141</v>
       </c>
       <c r="D11" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7921</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="1">
-        <v>140000</v>
+        <v>10000000</v>
       </c>
       <c r="B12" s="1">
-        <v>10</v>
+        <v>17031</v>
       </c>
       <c r="C12" s="1">
-        <v>0</v>
+        <v>2421</v>
       </c>
       <c r="D12" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>160000</v>
-      </c>
-      <c r="B13" s="1">
-        <v>11</v>
-      </c>
-      <c r="C13" s="1">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>180000</v>
-      </c>
-      <c r="B14" s="1">
-        <v>14</v>
-      </c>
-      <c r="C14" s="1">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>200000</v>
-      </c>
-      <c r="B15" s="1">
-        <v>14</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1">
-        <v>14</v>
+        <v>9133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>